<commit_message>
Se arregló las coordenadas negativas
</commit_message>
<xml_diff>
--- a/Coordenadas.xlsx
+++ b/Coordenadas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanj\Desktop\DERE\Tesis\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jodopevi/Documents/GitHub/Calculo_Distancias/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EA84C3D-655F-444F-9097-45014CA79021}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BF7326-6293-C449-8B0F-08B84C49E11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{7ACD5F33-3165-41CD-9F1D-8752AFB11E7E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="46080" windowHeight="24240" xr2:uid="{7ACD5F33-3165-41CD-9F1D-8752AFB11E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -781,17 +781,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3309C580-6DC3-4CD4-9740-A920BE6D1F6B}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -810,10 +807,10 @@
         <v>14.726699999999999</v>
       </c>
       <c r="C2">
-        <v>92.398399999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-92.398399999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -821,10 +818,10 @@
         <v>18.124400000000001</v>
       </c>
       <c r="C3">
-        <v>94.404200000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-94.404200000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -832,10 +829,10 @@
         <v>16.162500000000001</v>
       </c>
       <c r="C4">
-        <v>95.201400000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-95.201400000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -843,10 +840,10 @@
         <v>16.8184</v>
       </c>
       <c r="C5">
-        <v>99.185299999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.185299999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -854,10 +851,10 @@
         <v>17.934000000000001</v>
       </c>
       <c r="C6">
-        <v>102.1525</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.1525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -865,10 +862,10 @@
         <v>25.566700000000001</v>
       </c>
       <c r="C7">
-        <v>106.85590000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-106.85590000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -876,10 +873,10 @@
         <v>32.372900000000001</v>
       </c>
       <c r="C8">
-        <v>116.9404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-116.9404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -887,10 +884,10 @@
         <v>23.189900000000002</v>
       </c>
       <c r="C9">
-        <v>106.4362</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-106.4362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -898,10 +895,10 @@
         <v>19.0563</v>
       </c>
       <c r="C10">
-        <v>104.3167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.3167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -909,10 +906,10 @@
         <v>24.220199999999998</v>
       </c>
       <c r="C11">
-        <v>110.3052</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.3052</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -920,10 +917,10 @@
         <v>27.930199999999999</v>
       </c>
       <c r="C12">
-        <v>110.8489</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.8489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -931,10 +928,10 @@
         <v>19.210899999999999</v>
       </c>
       <c r="C13">
-        <v>96.130499999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.130499999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -942,10 +939,10 @@
         <v>19.813700000000001</v>
       </c>
       <c r="C14">
-        <v>90.554299999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-90.554299999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -953,10 +950,10 @@
         <v>21.221800000000002</v>
       </c>
       <c r="C15">
-        <v>89.618200000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-89.618200000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -964,10 +961,10 @@
         <v>17.995100000000001</v>
       </c>
       <c r="C16">
-        <v>92.973299999999995</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-92.973299999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -975,10 +972,10 @@
         <v>19.075800000000001</v>
       </c>
       <c r="C17">
-        <v>98.178899999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.178899999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -986,10 +983,10 @@
         <v>20.533300000000001</v>
       </c>
       <c r="C18">
-        <v>103.21510000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-103.21510000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -997,10 +994,10 @@
         <v>18.860700000000001</v>
       </c>
       <c r="C19">
-        <v>97.049300000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.049300000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1008,10 +1005,10 @@
         <v>18.442799999999998</v>
       </c>
       <c r="C20">
-        <v>96.343800000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.343800000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1019,10 +1016,10 @@
         <v>20.523900000000001</v>
       </c>
       <c r="C21">
-        <v>97.462500000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.462500000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1030,10 +1027,10 @@
         <v>20.711200000000002</v>
       </c>
       <c r="C22">
-        <v>103.46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-103.46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1041,10 +1038,10 @@
         <v>22.749700000000001</v>
       </c>
       <c r="C23">
-        <v>102.43819999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.43819999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1052,10 +1049,10 @@
         <v>22.1372</v>
       </c>
       <c r="C24">
-        <v>100.9956</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.9956</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1063,10 +1060,10 @@
         <v>19.464400000000001</v>
       </c>
       <c r="C25">
-        <v>99.201999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.201999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1074,10 +1071,10 @@
         <v>19.404599999999999</v>
       </c>
       <c r="C26">
-        <v>99.191400000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.191400000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1085,10 +1082,10 @@
         <v>18.921399999999998</v>
       </c>
       <c r="C27">
-        <v>99.197900000000004</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.197900000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1096,10 +1093,10 @@
         <v>19.527799999999999</v>
       </c>
       <c r="C28">
-        <v>99.110900000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.110900000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1107,10 +1104,10 @@
         <v>20.0946</v>
       </c>
       <c r="C29">
-        <v>98.706800000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.706800000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1118,10 +1115,10 @@
         <v>19.2881</v>
       </c>
       <c r="C30">
-        <v>99.583399999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.583399999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1129,10 +1126,10 @@
         <v>20.619700000000002</v>
       </c>
       <c r="C31">
-        <v>100.545</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.545</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1140,10 +1137,10 @@
         <v>20.520299999999999</v>
       </c>
       <c r="C32">
-        <v>100.7569</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.7569</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1151,10 +1148,10 @@
         <v>21.097000000000001</v>
       </c>
       <c r="C33">
-        <v>101.7152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.7152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1162,10 +1159,10 @@
         <v>19.840800000000002</v>
       </c>
       <c r="C34">
-        <v>101.42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1173,10 +1170,10 @@
         <v>20.630500000000001</v>
       </c>
       <c r="C35">
-        <v>101.1236</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.1236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1184,10 +1181,10 @@
         <v>21.757200000000001</v>
       </c>
       <c r="C36">
-        <v>102.2282</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.2282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1195,10 +1192,10 @@
         <v>19.365200000000002</v>
       </c>
       <c r="C37">
-        <v>99.277100000000004</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.277100000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1206,10 +1203,10 @@
         <v>25.702400000000001</v>
       </c>
       <c r="C38">
-        <v>100.49209999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.49209999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1217,10 +1214,10 @@
         <v>25.491</v>
       </c>
       <c r="C39">
-        <v>101.0003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.0003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1228,10 +1225,10 @@
         <v>27.849699999999999</v>
       </c>
       <c r="C40">
-        <v>100.75830000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.75830000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1239,10 +1236,10 @@
         <v>26.073599999999999</v>
       </c>
       <c r="C41">
-        <v>98.369100000000003</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.369100000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1250,10 +1247,10 @@
         <v>26.964500000000001</v>
       </c>
       <c r="C42">
-        <v>101.5444</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.5444</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1261,10 +1258,10 @@
         <v>25.563199999999998</v>
       </c>
       <c r="C43">
-        <v>103.08620000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-103.08620000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1272,10 +1269,10 @@
         <v>28.597100000000001</v>
       </c>
       <c r="C44">
-        <v>105.9881</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-105.9881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1283,10 +1280,10 @@
         <v>23.686800000000002</v>
       </c>
       <c r="C45">
-        <v>99.093999999999994</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.093999999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1294,10 +1291,10 @@
         <v>20.0837</v>
       </c>
       <c r="C46">
-        <v>102.4072</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.4072</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1305,10 +1302,10 @@
         <v>25.595300000000002</v>
       </c>
       <c r="C47">
-        <v>100.00320000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.00320000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1316,10 +1313,10 @@
         <v>31.607399999999998</v>
       </c>
       <c r="C48">
-        <v>106.49420000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-106.49420000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1327,10 +1324,10 @@
         <v>16.217500000000001</v>
       </c>
       <c r="C49">
-        <v>95.183499999999995</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-95.183499999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1338,10 +1335,10 @@
         <v>29.023299999999999</v>
       </c>
       <c r="C50">
-        <v>110.8878</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.8878</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1349,10 +1346,10 @@
         <v>17.9878</v>
       </c>
       <c r="C51">
-        <v>94.592100000000002</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-94.592100000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1360,10 +1357,10 @@
         <v>31.884499999999999</v>
       </c>
       <c r="C52">
-        <v>116.47790000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-116.47790000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1371,10 +1368,10 @@
         <v>32.5807</v>
       </c>
       <c r="C53">
-        <v>115.6397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-115.6397</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1382,10 +1379,10 @@
         <v>27.544599999999999</v>
       </c>
       <c r="C54">
-        <v>109.8754</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-109.8754</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1393,10 +1390,10 @@
         <v>24.769100000000002</v>
       </c>
       <c r="C55">
-        <v>107.5778</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-107.5778</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1404,10 +1401,10 @@
         <v>25.471699999999998</v>
       </c>
       <c r="C56">
-        <v>108.0829</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-108.0829</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1415,10 +1412,10 @@
         <v>20.924800000000001</v>
       </c>
       <c r="C57">
-        <v>89.683599999999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-89.683599999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1426,10 +1423,10 @@
         <v>27.030799999999999</v>
       </c>
       <c r="C58">
-        <v>109.4308</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-109.4308</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1437,10 +1434,10 @@
         <v>30.638200000000001</v>
       </c>
       <c r="C59">
-        <v>110.96339999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.96339999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1448,10 +1445,10 @@
         <v>19.5717</v>
       </c>
       <c r="C60">
-        <v>96.926500000000004</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.926500000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1459,10 +1456,10 @@
         <v>21.481999999999999</v>
       </c>
       <c r="C61">
-        <v>104.82340000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.82340000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1470,10 +1467,10 @@
         <v>19.234400000000001</v>
       </c>
       <c r="C62">
-        <v>103.767</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-103.767</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1481,10 +1478,10 @@
         <v>26.9831</v>
       </c>
       <c r="C63">
-        <v>105.6602</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-105.6602</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1492,10 +1489,10 @@
         <v>27.492699999999999</v>
       </c>
       <c r="C64">
-        <v>99.569900000000004</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.569900000000004</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -1503,10 +1500,10 @@
         <v>23.666</v>
       </c>
       <c r="C65">
-        <v>100.6435</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.6435</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -1514,10 +1511,10 @@
         <v>18.753900000000002</v>
       </c>
       <c r="C66">
-        <v>98.906199999999998</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.906199999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -1525,10 +1522,10 @@
         <v>18.359400000000001</v>
       </c>
       <c r="C67">
-        <v>99.536299999999997</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.536299999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -1536,10 +1533,10 @@
         <v>19.421399999999998</v>
       </c>
       <c r="C68">
-        <v>102.0005</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.0005</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -1547,10 +1544,10 @@
         <v>22.7103</v>
       </c>
       <c r="C69">
-        <v>98.981700000000004</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.981700000000004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -1558,10 +1555,10 @@
         <v>19.570900000000002</v>
       </c>
       <c r="C70">
-        <v>97.250799999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.250799999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -1569,10 +1566,10 @@
         <v>17.033799999999999</v>
       </c>
       <c r="C71">
-        <v>96.611599999999996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.611599999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -1580,10 +1577,10 @@
         <v>16.765599999999999</v>
       </c>
       <c r="C72">
-        <v>93.1935</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-93.1935</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -1591,10 +1588,10 @@
         <v>22.0062</v>
       </c>
       <c r="C73">
-        <v>99.037700000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.037700000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -1602,10 +1599,10 @@
         <v>24.032499999999999</v>
       </c>
       <c r="C74">
-        <v>104.626</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.626</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -1613,10 +1610,10 @@
         <v>18.541499999999999</v>
       </c>
       <c r="C75">
-        <v>97.431899999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.431899999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -1624,10 +1621,10 @@
         <v>31.279699999999998</v>
       </c>
       <c r="C76">
-        <v>110.9367</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.9367</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -1635,10 +1632,10 @@
         <v>22.258800000000001</v>
       </c>
       <c r="C77">
-        <v>97.809399999999997</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.809399999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -1646,10 +1643,10 @@
         <v>20.973400000000002</v>
       </c>
       <c r="C78">
-        <v>97.317400000000006</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.317400000000006</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -1657,10 +1654,10 @@
         <v>20.961400000000001</v>
       </c>
       <c r="C79">
-        <v>97.3172</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.3172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -1668,10 +1665,10 @@
         <v>19.215699999999998</v>
       </c>
       <c r="C80">
-        <v>96.137299999999996</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.137299999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -1679,10 +1676,10 @@
         <v>22.030899999999999</v>
       </c>
       <c r="C81">
-        <v>100.8999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.8999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -1690,10 +1687,10 @@
         <v>21.044899999999998</v>
       </c>
       <c r="C82">
-        <v>100.47199999999999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.47199999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -1701,10 +1698,10 @@
         <v>19.610399999999998</v>
       </c>
       <c r="C83">
-        <v>98.955600000000004</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.955600000000004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -1712,10 +1709,10 @@
         <v>21.319800000000001</v>
       </c>
       <c r="C84">
-        <v>101.9186</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.9186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -1723,10 +1720,10 @@
         <v>25.8856</v>
       </c>
       <c r="C85">
-        <v>97.528199999999998</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.528199999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -1734,10 +1731,10 @@
         <v>19.026900000000001</v>
       </c>
       <c r="C86">
-        <v>104.32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -1745,10 +1742,10 @@
         <v>19.462299999999999</v>
       </c>
       <c r="C87">
-        <v>99.158600000000007</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.158600000000007</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -1756,10 +1753,10 @@
         <v>20.944199999999999</v>
       </c>
       <c r="C88">
-        <v>97.331400000000002</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.331400000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -1767,10 +1764,10 @@
         <v>22.5029</v>
       </c>
       <c r="C89">
-        <v>97.896799999999999</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.896799999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -1778,10 +1775,10 @@
         <v>32.534399999999998</v>
       </c>
       <c r="C90">
-        <v>115.3441</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-115.3441</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -1789,10 +1786,10 @@
         <v>25.8246</v>
       </c>
       <c r="C91">
-        <v>100.3424</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.3424</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -1800,10 +1797,10 @@
         <v>19.648900000000001</v>
       </c>
       <c r="C92">
-        <v>99.811000000000007</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.811000000000007</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -1811,10 +1808,10 @@
         <v>26.027100000000001</v>
       </c>
       <c r="C93">
-        <v>98.469899999999996</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.469899999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -1822,10 +1819,10 @@
         <v>28.529800000000002</v>
       </c>
       <c r="C94">
-        <v>105.95350000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-105.95350000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -1833,10 +1830,10 @@
         <v>19.749500000000001</v>
       </c>
       <c r="C95">
-        <v>98.649900000000002</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.649900000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -1844,10 +1841,10 @@
         <v>19.245100000000001</v>
       </c>
       <c r="C96">
-        <v>96.175299999999993</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-96.175299999999993</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -1855,10 +1852,10 @@
         <v>19.9178</v>
       </c>
       <c r="C97">
-        <v>99.244</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.244</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>99</v>
       </c>
@@ -1866,10 +1863,10 @@
         <v>29.244199999999999</v>
       </c>
       <c r="C98">
-        <v>110.8918</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-110.8918</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -1877,10 +1874,10 @@
         <v>19.0061</v>
       </c>
       <c r="C99">
-        <v>104.2496</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.2496</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -1888,10 +1885,10 @@
         <v>19.777200000000001</v>
       </c>
       <c r="C100">
-        <v>99.871899999999997</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.871899999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -1899,10 +1896,10 @@
         <v>20.950900000000001</v>
       </c>
       <c r="C101">
-        <v>97.327799999999996</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.327799999999996</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -1910,10 +1907,10 @@
         <v>22.395399999999999</v>
       </c>
       <c r="C102">
-        <v>102.2911</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-102.2911</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -1921,10 +1918,10 @@
         <v>26.0167</v>
       </c>
       <c r="C103">
-        <v>100.297</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-100.297</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -1932,10 +1929,10 @@
         <v>18.434200000000001</v>
       </c>
       <c r="C104">
-        <v>93.196899999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-93.196899999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -1943,10 +1940,10 @@
         <v>19.016500000000001</v>
       </c>
       <c r="C105">
-        <v>104.2863</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-104.2863</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -1954,10 +1951,10 @@
         <v>21.348600000000001</v>
       </c>
       <c r="C106">
-        <v>89.6798</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-89.6798</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>108</v>
       </c>
@@ -1965,10 +1962,10 @@
         <v>22.4773</v>
       </c>
       <c r="C107">
-        <v>97.865300000000005</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.865300000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -1976,10 +1973,10 @@
         <v>19.836099999999998</v>
       </c>
       <c r="C108">
-        <v>98.927499999999995</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.927499999999995</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -1987,10 +1984,10 @@
         <v>19.202400000000001</v>
       </c>
       <c r="C109">
-        <v>98.359800000000007</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.359800000000007</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -1998,10 +1995,10 @@
         <v>22.497900000000001</v>
       </c>
       <c r="C110">
-        <v>97.893799999999999</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.893799999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>112</v>
       </c>
@@ -2009,10 +2006,10 @@
         <v>25.5886</v>
       </c>
       <c r="C111">
-        <v>99.944400000000002</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.944400000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -2020,10 +2017,10 @@
         <v>20.043199999999999</v>
       </c>
       <c r="C112">
-        <v>99.271799999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-99.271799999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>114</v>
       </c>
@@ -2031,10 +2028,10 @@
         <v>20.5794</v>
       </c>
       <c r="C113">
-        <v>101.1781</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-101.1781</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -2042,10 +2039,10 @@
         <v>22.275500000000001</v>
       </c>
       <c r="C114">
-        <v>97.813299999999998</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-97.813299999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>116</v>
       </c>
@@ -2053,10 +2050,10 @@
         <v>17.970800000000001</v>
       </c>
       <c r="C115">
-        <v>94.533799999999999</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-94.533799999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -2064,10 +2061,10 @@
         <v>16.211500000000001</v>
       </c>
       <c r="C116">
-        <v>95.179500000000004</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-95.179500000000004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -2075,10 +2072,10 @@
         <v>33.772599999999997</v>
       </c>
       <c r="C117">
-        <v>118.2308</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-118.2308</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>119</v>
       </c>
@@ -2086,10 +2083,10 @@
         <v>31.770299999999999</v>
       </c>
       <c r="C118">
-        <v>106.3991</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-106.3991</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -2097,10 +2094,10 @@
         <v>29.348299999999998</v>
       </c>
       <c r="C119">
-        <v>98.459500000000006</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+        <v>-98.459500000000006</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -2108,7 +2105,7 @@
         <v>28.456399999999999</v>
       </c>
       <c r="C120">
-        <v>98.179199999999994</v>
+        <v>-98.179199999999994</v>
       </c>
     </row>
   </sheetData>
@@ -2125,9 +2122,9 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2147,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2161,7 +2158,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2174,7 +2171,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2189,12 +2186,12 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>123</v>
       </c>

</xml_diff>